<commit_message>
Add mapping mos (#250)
* add mapping mos

* add mapping

* update device mapping

* add errors

* svs

* rm deprecated pattern

* update

* update

* update mappings 5423cc8d0d2f6ad99a507aa3c1ad050a5a4c88c5
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-as-cs-type-etablissement.xlsx
+++ b/main/ig/CodeSystem-as-cs-type-etablissement.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-02T14:05:36+00:00</t>
+    <t>2025-01-15T07:47:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Case Sensitive</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
   <si>
     <t>Value Set (all codes)</t>
@@ -409,52 +412,54 @@
       <c r="A15" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" t="s" s="2">
+        <v>27</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -472,44 +477,44 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>